<commit_message>
fix descr add top3
</commit_message>
<xml_diff>
--- a/descr4.xlsx
+++ b/descr4.xlsx
@@ -3605,7 +3605,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -3652,28 +3652,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="11"/>
       </left>
       <right style="thin">
@@ -3691,24 +3669,6 @@
       <left style="thin">
         <color indexed="11"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -3718,15 +3678,6 @@
       <bottom style="thin">
         <color indexed="11"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -3813,15 +3764,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="11"/>
       </left>
       <right style="thin">
@@ -3878,35 +3820,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -3922,107 +3842,83 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" readingOrder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5109,7 +5005,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -5118,8 +5014,7 @@
     <col min="1" max="1" width="35.8516" style="1" customWidth="1"/>
     <col min="2" max="2" width="56.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="96.1719" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85156" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="61.75" customHeight="1">
@@ -5132,1295 +5027,1095 @@
       <c r="C1" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
     </row>
     <row r="2" ht="206.75" customHeight="1">
-      <c r="A2" t="s" s="7">
+      <c r="A2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="B2" t="s" s="8">
+      <c r="B2" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="9">
+      <c r="C2" t="s" s="7">
         <v>5</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
     </row>
     <row r="3" ht="106.5" customHeight="1">
-      <c r="A3" t="s" s="7">
+      <c r="A3" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="B3" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="9">
+      <c r="C3" t="s" s="7">
         <v>8</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
     </row>
     <row r="4" ht="54.5" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="A4" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="8">
+      <c r="B4" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="12">
+      <c r="C4" t="s" s="8">
         <v>11</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
     </row>
     <row r="5" ht="31.75" customHeight="1">
-      <c r="A5" t="s" s="7">
+      <c r="A5" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="B5" t="s" s="8">
+      <c r="B5" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="C5" t="s" s="8">
+      <c r="C5" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
     </row>
     <row r="6" ht="31.5" customHeight="1">
-      <c r="A6" t="s" s="7">
+      <c r="A6" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="B6" t="s" s="8">
+      <c r="B6" t="s" s="6">
         <v>16</v>
       </c>
-      <c r="C6" t="s" s="8">
+      <c r="C6" t="s" s="6">
         <v>17</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
     </row>
     <row r="7" ht="31.5" customHeight="1">
-      <c r="A7" t="s" s="7">
+      <c r="A7" t="s" s="5">
         <v>18</v>
       </c>
-      <c r="B7" t="s" s="8">
+      <c r="B7" t="s" s="6">
         <v>19</v>
       </c>
-      <c r="C7" t="s" s="13">
+      <c r="C7" t="s" s="9">
         <v>20</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
     </row>
     <row r="8" ht="54.5" customHeight="1">
-      <c r="A8" t="s" s="7">
+      <c r="A8" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="B8" t="s" s="8">
+      <c r="B8" t="s" s="6">
         <v>22</v>
       </c>
-      <c r="C8" t="s" s="14">
+      <c r="C8" t="s" s="10">
         <v>23</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
     </row>
     <row r="9" ht="54.5" customHeight="1">
-      <c r="A9" t="s" s="7">
+      <c r="A9" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="B9" t="s" s="8">
+      <c r="B9" t="s" s="6">
         <v>25</v>
       </c>
-      <c r="C9" t="s" s="12">
+      <c r="C9" t="s" s="8">
         <v>26</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
     </row>
     <row r="10" ht="31.5" customHeight="1">
-      <c r="A10" t="s" s="7">
+      <c r="A10" t="s" s="5">
         <v>27</v>
       </c>
-      <c r="B10" t="s" s="8">
+      <c r="B10" t="s" s="6">
         <v>28</v>
       </c>
-      <c r="C10" t="s" s="13">
+      <c r="C10" t="s" s="9">
         <v>20</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
     </row>
     <row r="11" ht="31.5" customHeight="1">
-      <c r="A11" t="s" s="7">
+      <c r="A11" t="s" s="5">
         <v>29</v>
       </c>
-      <c r="B11" t="s" s="8">
+      <c r="B11" t="s" s="6">
         <v>30</v>
       </c>
-      <c r="C11" t="s" s="15">
+      <c r="C11" t="s" s="11">
         <v>31</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
     </row>
     <row r="12" ht="129.75" customHeight="1">
-      <c r="A12" t="s" s="7">
+      <c r="A12" t="s" s="5">
         <v>32</v>
       </c>
-      <c r="B12" t="s" s="8">
+      <c r="B12" t="s" s="6">
         <v>33</v>
       </c>
-      <c r="C12" t="s" s="9">
+      <c r="C12" t="s" s="7">
         <v>34</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
     </row>
     <row r="13" ht="54.75" customHeight="1">
-      <c r="A13" t="s" s="7">
+      <c r="A13" t="s" s="5">
         <v>35</v>
       </c>
-      <c r="B13" t="s" s="8">
+      <c r="B13" t="s" s="6">
         <v>36</v>
       </c>
-      <c r="C13" t="s" s="9">
+      <c r="C13" t="s" s="7">
         <v>37</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
     </row>
     <row r="14" ht="31.5" customHeight="1">
-      <c r="A14" t="s" s="7">
+      <c r="A14" t="s" s="5">
         <v>38</v>
       </c>
-      <c r="B14" t="s" s="8">
+      <c r="B14" t="s" s="6">
         <v>39</v>
       </c>
-      <c r="C14" t="s" s="8">
+      <c r="C14" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
     </row>
     <row r="15" ht="77.75" customHeight="1">
-      <c r="A15" t="s" s="7">
+      <c r="A15" t="s" s="5">
         <v>41</v>
       </c>
-      <c r="B15" t="s" s="8">
+      <c r="B15" t="s" s="6">
         <v>42</v>
       </c>
-      <c r="C15" t="s" s="16">
+      <c r="C15" t="s" s="12">
         <v>43</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
     </row>
     <row r="16" ht="54.5" customHeight="1">
-      <c r="A16" t="s" s="7">
+      <c r="A16" t="s" s="5">
         <v>44</v>
       </c>
-      <c r="B16" t="s" s="8">
+      <c r="B16" t="s" s="6">
         <v>45</v>
       </c>
-      <c r="C16" t="s" s="16">
+      <c r="C16" t="s" s="12">
         <v>46</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
     </row>
     <row r="17" ht="31.5" customHeight="1">
-      <c r="A17" t="s" s="7">
+      <c r="A17" t="s" s="5">
         <v>47</v>
       </c>
-      <c r="B17" t="s" s="8">
+      <c r="B17" t="s" s="6">
         <v>48</v>
       </c>
-      <c r="C17" t="s" s="15">
+      <c r="C17" t="s" s="11">
         <v>49</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
     </row>
     <row r="18" ht="77.75" customHeight="1">
-      <c r="A18" t="s" s="7">
+      <c r="A18" t="s" s="5">
         <v>50</v>
       </c>
-      <c r="B18" t="s" s="8">
+      <c r="B18" t="s" s="6">
         <v>51</v>
       </c>
-      <c r="C18" t="s" s="17">
+      <c r="C18" t="s" s="13">
         <v>52</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="11"/>
     </row>
     <row r="19" ht="77.5" customHeight="1">
-      <c r="A19" t="s" s="7">
+      <c r="A19" t="s" s="5">
         <v>53</v>
       </c>
-      <c r="B19" t="s" s="8">
+      <c r="B19" t="s" s="6">
         <v>54</v>
       </c>
-      <c r="C19" t="s" s="16">
+      <c r="C19" t="s" s="12">
         <v>55</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
     </row>
     <row r="20" ht="77.75" customHeight="1">
-      <c r="A20" t="s" s="7">
+      <c r="A20" t="s" s="5">
         <v>56</v>
       </c>
-      <c r="B20" t="s" s="8">
+      <c r="B20" t="s" s="6">
         <v>57</v>
       </c>
-      <c r="C20" t="s" s="16">
+      <c r="C20" t="s" s="12">
         <v>43</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
     </row>
     <row r="21" ht="69.75" customHeight="1">
-      <c r="A21" t="s" s="7">
+      <c r="A21" t="s" s="5">
         <v>58</v>
       </c>
-      <c r="B21" t="s" s="8">
+      <c r="B21" t="s" s="6">
         <v>59</v>
       </c>
-      <c r="C21" t="s" s="19">
+      <c r="C21" t="s" s="14">
         <v>60</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="11"/>
     </row>
     <row r="22" ht="69.5" customHeight="1">
-      <c r="A22" t="s" s="7">
+      <c r="A22" t="s" s="5">
         <v>61</v>
       </c>
-      <c r="B22" t="s" s="8">
+      <c r="B22" t="s" s="6">
         <v>62</v>
       </c>
-      <c r="C22" t="s" s="16">
+      <c r="C22" t="s" s="12">
         <v>63</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
     </row>
     <row r="23" ht="46.5" customHeight="1">
-      <c r="A23" t="s" s="7">
+      <c r="A23" t="s" s="5">
         <v>64</v>
       </c>
-      <c r="B23" t="s" s="8">
+      <c r="B23" t="s" s="6">
         <v>65</v>
       </c>
-      <c r="C23" t="s" s="15">
+      <c r="C23" t="s" s="11">
         <v>66</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
     </row>
     <row r="24" ht="54.75" customHeight="1">
-      <c r="A24" t="s" s="7">
+      <c r="A24" t="s" s="5">
         <v>67</v>
       </c>
-      <c r="B24" t="s" s="8">
+      <c r="B24" t="s" s="6">
         <v>68</v>
       </c>
-      <c r="C24" t="s" s="15">
+      <c r="C24" t="s" s="11">
         <v>69</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
     </row>
     <row r="25" ht="31.5" customHeight="1">
-      <c r="A25" t="s" s="7">
+      <c r="A25" t="s" s="5">
         <v>70</v>
       </c>
-      <c r="B25" t="s" s="8">
+      <c r="B25" t="s" s="6">
         <v>71</v>
       </c>
-      <c r="C25" t="s" s="20">
+      <c r="C25" t="s" s="15">
         <v>72</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="11"/>
     </row>
     <row r="26" ht="31.5" customHeight="1">
-      <c r="A26" t="s" s="7">
+      <c r="A26" t="s" s="5">
         <v>73</v>
       </c>
-      <c r="B26" t="s" s="8">
+      <c r="B26" t="s" s="6">
         <v>74</v>
       </c>
-      <c r="C26" t="s" s="15">
+      <c r="C26" t="s" s="11">
         <v>75</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
     </row>
     <row r="27" ht="69.75" customHeight="1">
-      <c r="A27" t="s" s="7">
+      <c r="A27" t="s" s="5">
         <v>76</v>
       </c>
-      <c r="B27" t="s" s="8">
+      <c r="B27" t="s" s="6">
         <v>59</v>
       </c>
-      <c r="C27" t="s" s="16">
+      <c r="C27" t="s" s="12">
         <v>77</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11"/>
     </row>
     <row r="28" ht="69.75" customHeight="1">
-      <c r="A28" t="s" s="7">
+      <c r="A28" t="s" s="5">
         <v>78</v>
       </c>
-      <c r="B28" t="s" s="8">
+      <c r="B28" t="s" s="6">
         <v>59</v>
       </c>
-      <c r="C28" t="s" s="15">
+      <c r="C28" t="s" s="11">
         <v>79</v>
       </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="11"/>
     </row>
     <row r="29" ht="409.5" customHeight="1">
-      <c r="A29" t="s" s="7">
+      <c r="A29" t="s" s="5">
         <v>80</v>
       </c>
-      <c r="B29" t="s" s="8">
+      <c r="B29" t="s" s="6">
         <v>81</v>
       </c>
-      <c r="C29" t="s" s="9">
+      <c r="C29" t="s" s="7">
         <v>82</v>
       </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="11"/>
     </row>
     <row r="30" ht="31.5" customHeight="1">
-      <c r="A30" t="s" s="7">
+      <c r="A30" t="s" s="5">
         <v>83</v>
       </c>
-      <c r="B30" t="s" s="8">
+      <c r="B30" t="s" s="6">
         <v>84</v>
       </c>
-      <c r="C30" t="s" s="8">
+      <c r="C30" t="s" s="6">
         <v>85</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="11"/>
     </row>
     <row r="31" ht="54.75" customHeight="1">
-      <c r="A31" t="s" s="7">
+      <c r="A31" t="s" s="5">
         <v>86</v>
       </c>
-      <c r="B31" t="s" s="8">
+      <c r="B31" t="s" s="6">
         <v>87</v>
       </c>
-      <c r="C31" t="s" s="15">
+      <c r="C31" t="s" s="11">
         <v>88</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="11"/>
     </row>
     <row r="32" ht="409.5" customHeight="1">
-      <c r="A32" t="s" s="7">
+      <c r="A32" t="s" s="5">
         <v>89</v>
       </c>
-      <c r="B32" t="s" s="8">
+      <c r="B32" t="s" s="6">
         <v>90</v>
       </c>
-      <c r="C32" t="s" s="16">
+      <c r="C32" t="s" s="12">
         <v>82</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="11"/>
     </row>
     <row r="33" ht="54.75" customHeight="1">
-      <c r="A33" t="s" s="7">
+      <c r="A33" t="s" s="5">
         <v>91</v>
       </c>
-      <c r="B33" t="s" s="8">
+      <c r="B33" t="s" s="6">
         <v>92</v>
       </c>
-      <c r="C33" t="s" s="15">
+      <c r="C33" t="s" s="11">
         <v>93</v>
       </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="11"/>
     </row>
     <row r="34" ht="54.75" customHeight="1">
-      <c r="A34" t="s" s="7">
+      <c r="A34" t="s" s="5">
         <v>94</v>
       </c>
-      <c r="B34" t="s" s="8">
+      <c r="B34" t="s" s="6">
         <v>95</v>
       </c>
-      <c r="C34" t="s" s="15">
+      <c r="C34" t="s" s="11">
         <v>96</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="11"/>
     </row>
     <row r="35" ht="31.5" customHeight="1">
-      <c r="A35" t="s" s="7">
+      <c r="A35" t="s" s="5">
         <v>97</v>
       </c>
-      <c r="B35" t="s" s="8">
+      <c r="B35" t="s" s="6">
         <v>98</v>
       </c>
-      <c r="C35" t="s" s="8">
+      <c r="C35" t="s" s="6">
         <v>99</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="11"/>
     </row>
     <row r="36" ht="200.75" customHeight="1">
-      <c r="A36" t="s" s="7">
+      <c r="A36" t="s" s="5">
         <v>100</v>
       </c>
-      <c r="B36" t="s" s="8">
+      <c r="B36" t="s" s="6">
         <v>101</v>
       </c>
-      <c r="C36" t="s" s="16">
+      <c r="C36" t="s" s="12">
         <v>102</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="11"/>
     </row>
     <row r="37" ht="77.75" customHeight="1">
-      <c r="A37" t="s" s="7">
+      <c r="A37" t="s" s="5">
         <v>103</v>
       </c>
-      <c r="B37" t="s" s="8">
+      <c r="B37" t="s" s="6">
         <v>104</v>
       </c>
-      <c r="C37" t="s" s="16">
+      <c r="C37" t="s" s="12">
         <v>105</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
     </row>
     <row r="38" ht="54.75" customHeight="1">
-      <c r="A38" t="s" s="7">
+      <c r="A38" t="s" s="5">
         <v>106</v>
       </c>
-      <c r="B38" t="s" s="8">
+      <c r="B38" t="s" s="6">
         <v>107</v>
       </c>
-      <c r="C38" t="s" s="16">
+      <c r="C38" t="s" s="12">
         <v>108</v>
       </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
     </row>
     <row r="39" ht="77.75" customHeight="1">
-      <c r="A39" t="s" s="7">
+      <c r="A39" t="s" s="5">
         <v>109</v>
       </c>
-      <c r="B39" t="s" s="8">
+      <c r="B39" t="s" s="6">
         <v>110</v>
       </c>
-      <c r="C39" t="s" s="16">
+      <c r="C39" t="s" s="12">
         <v>111</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="11"/>
     </row>
     <row r="40" ht="54.75" customHeight="1">
-      <c r="A40" t="s" s="7">
+      <c r="A40" t="s" s="5">
         <v>112</v>
       </c>
-      <c r="B40" t="s" s="8">
+      <c r="B40" t="s" s="6">
         <v>113</v>
       </c>
-      <c r="C40" t="s" s="16">
+      <c r="C40" t="s" s="12">
         <v>114</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="11"/>
     </row>
     <row r="41" ht="54.75" customHeight="1">
-      <c r="A41" t="s" s="7">
+      <c r="A41" t="s" s="5">
         <v>115</v>
       </c>
-      <c r="B41" t="s" s="8">
+      <c r="B41" t="s" s="6">
         <v>116</v>
       </c>
-      <c r="C41" t="s" s="16">
+      <c r="C41" t="s" s="12">
         <v>117</v>
       </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
     </row>
     <row r="42" ht="77.75" customHeight="1">
-      <c r="A42" t="s" s="7">
+      <c r="A42" t="s" s="5">
         <v>118</v>
       </c>
-      <c r="B42" t="s" s="8">
+      <c r="B42" t="s" s="6">
         <v>119</v>
       </c>
-      <c r="C42" t="s" s="16">
+      <c r="C42" t="s" s="12">
         <v>120</v>
       </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="11"/>
     </row>
     <row r="43" ht="77.5" customHeight="1">
-      <c r="A43" t="s" s="7">
+      <c r="A43" t="s" s="5">
         <v>121</v>
       </c>
-      <c r="B43" t="s" s="8">
+      <c r="B43" t="s" s="6">
         <v>122</v>
       </c>
-      <c r="C43" t="s" s="17">
+      <c r="C43" t="s" s="13">
         <v>123</v>
       </c>
-      <c r="D43" s="18"/>
-      <c r="E43" s="11"/>
     </row>
     <row r="44" ht="54.75" customHeight="1">
-      <c r="A44" t="s" s="7">
+      <c r="A44" t="s" s="5">
         <v>124</v>
       </c>
-      <c r="B44" t="s" s="8">
+      <c r="B44" t="s" s="6">
         <v>125</v>
       </c>
-      <c r="C44" t="s" s="15">
+      <c r="C44" t="s" s="11">
         <v>126</v>
       </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="11"/>
     </row>
     <row r="45" ht="54.75" customHeight="1">
-      <c r="A45" t="s" s="7">
+      <c r="A45" t="s" s="5">
         <v>127</v>
       </c>
-      <c r="B45" t="s" s="8">
+      <c r="B45" t="s" s="6">
         <v>128</v>
       </c>
-      <c r="C45" t="s" s="15">
+      <c r="C45" t="s" s="11">
         <v>129</v>
       </c>
-      <c r="D45" s="10"/>
-      <c r="E45" s="11"/>
     </row>
     <row r="46" ht="54.75" customHeight="1">
-      <c r="A46" t="s" s="7">
+      <c r="A46" t="s" s="5">
         <v>130</v>
       </c>
-      <c r="B46" t="s" s="8">
+      <c r="B46" t="s" s="6">
         <v>131</v>
       </c>
-      <c r="C46" t="s" s="16">
+      <c r="C46" t="s" s="12">
         <v>132</v>
       </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="11"/>
     </row>
     <row r="47" ht="100.75" customHeight="1">
-      <c r="A47" t="s" s="7">
+      <c r="A47" t="s" s="5">
         <v>133</v>
       </c>
-      <c r="B47" t="s" s="8">
+      <c r="B47" t="s" s="6">
         <v>134</v>
       </c>
-      <c r="C47" t="s" s="16">
+      <c r="C47" t="s" s="12">
         <v>135</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="11"/>
     </row>
     <row r="48" ht="54.75" customHeight="1">
-      <c r="A48" t="s" s="7">
+      <c r="A48" t="s" s="5">
         <v>136</v>
       </c>
-      <c r="B48" t="s" s="8">
+      <c r="B48" t="s" s="6">
         <v>137</v>
       </c>
-      <c r="C48" t="s" s="16">
+      <c r="C48" t="s" s="12">
         <v>43</v>
       </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="11"/>
     </row>
     <row r="49" ht="31.75" customHeight="1">
-      <c r="A49" t="s" s="7">
+      <c r="A49" t="s" s="5">
         <v>138</v>
       </c>
-      <c r="B49" t="s" s="8">
+      <c r="B49" t="s" s="6">
         <v>139</v>
       </c>
-      <c r="C49" t="s" s="8">
+      <c r="C49" t="s" s="6">
         <v>140</v>
       </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="11"/>
     </row>
     <row r="50" ht="77.75" customHeight="1">
-      <c r="A50" t="s" s="7">
+      <c r="A50" t="s" s="5">
         <v>141</v>
       </c>
-      <c r="B50" t="s" s="21">
+      <c r="B50" t="s" s="16">
         <v>142</v>
       </c>
-      <c r="C50" t="s" s="16">
+      <c r="C50" t="s" s="12">
         <v>143</v>
       </c>
-      <c r="D50" s="10"/>
-      <c r="E50" s="11"/>
     </row>
     <row r="51" ht="31.5" customHeight="1">
-      <c r="A51" t="s" s="7">
+      <c r="A51" t="s" s="5">
         <v>144</v>
       </c>
-      <c r="B51" t="s" s="8">
+      <c r="B51" t="s" s="6">
         <v>145</v>
       </c>
-      <c r="C51" t="s" s="15">
+      <c r="C51" t="s" s="11">
         <v>146</v>
       </c>
-      <c r="D51" s="10"/>
-      <c r="E51" s="11"/>
     </row>
     <row r="52" ht="31.5" customHeight="1">
-      <c r="A52" t="s" s="7">
+      <c r="A52" t="s" s="5">
         <v>147</v>
       </c>
-      <c r="B52" t="s" s="8">
+      <c r="B52" t="s" s="6">
         <v>148</v>
       </c>
-      <c r="C52" t="s" s="22">
+      <c r="C52" t="s" s="17">
         <v>149</v>
       </c>
-      <c r="D52" s="18"/>
-      <c r="E52" s="11"/>
     </row>
     <row r="53" ht="69.75" customHeight="1">
-      <c r="A53" t="s" s="7">
+      <c r="A53" t="s" s="5">
         <v>150</v>
       </c>
-      <c r="B53" t="s" s="8">
+      <c r="B53" t="s" s="6">
         <v>59</v>
       </c>
-      <c r="C53" t="s" s="23">
+      <c r="C53" t="s" s="18">
         <v>151</v>
       </c>
-      <c r="D53" s="18"/>
-      <c r="E53" s="11"/>
     </row>
     <row r="54" ht="54.75" customHeight="1">
-      <c r="A54" t="s" s="7">
+      <c r="A54" t="s" s="5">
         <v>152</v>
       </c>
-      <c r="B54" t="s" s="8">
+      <c r="B54" t="s" s="6">
         <v>153</v>
       </c>
-      <c r="C54" t="s" s="24">
+      <c r="C54" t="s" s="19">
         <v>154</v>
       </c>
-      <c r="D54" s="18"/>
-      <c r="E54" s="11"/>
     </row>
     <row r="55" ht="31.5" customHeight="1">
-      <c r="A55" t="s" s="7">
+      <c r="A55" t="s" s="5">
         <v>155</v>
       </c>
-      <c r="B55" t="s" s="8">
+      <c r="B55" t="s" s="6">
         <v>156</v>
       </c>
-      <c r="C55" t="s" s="13">
+      <c r="C55" t="s" s="9">
         <v>157</v>
       </c>
-      <c r="D55" s="10"/>
-      <c r="E55" s="11"/>
     </row>
     <row r="56" ht="31.5" customHeight="1">
-      <c r="A56" t="s" s="7">
+      <c r="A56" t="s" s="5">
         <v>158</v>
       </c>
-      <c r="B56" t="s" s="8">
+      <c r="B56" t="s" s="6">
         <v>159</v>
       </c>
-      <c r="C56" t="s" s="8">
+      <c r="C56" t="s" s="6">
         <v>160</v>
       </c>
-      <c r="D56" s="10"/>
-      <c r="E56" s="11"/>
     </row>
     <row r="57" ht="287.5" customHeight="1">
-      <c r="A57" t="s" s="7">
+      <c r="A57" t="s" s="5">
         <v>161</v>
       </c>
-      <c r="B57" t="s" s="8">
+      <c r="B57" t="s" s="6">
         <v>162</v>
       </c>
-      <c r="C57" t="s" s="25">
+      <c r="C57" t="s" s="20">
         <v>163</v>
       </c>
-      <c r="D57" s="10"/>
-      <c r="E57" s="11"/>
     </row>
     <row r="58" ht="77.75" customHeight="1">
-      <c r="A58" t="s" s="7">
+      <c r="A58" t="s" s="5">
         <v>164</v>
       </c>
-      <c r="B58" t="s" s="26">
+      <c r="B58" t="s" s="21">
         <v>165</v>
       </c>
-      <c r="C58" t="s" s="27">
+      <c r="C58" t="s" s="22">
         <v>166</v>
       </c>
-      <c r="D58" s="28"/>
-      <c r="E58" s="11"/>
     </row>
     <row r="59" ht="77.75" customHeight="1">
-      <c r="A59" t="s" s="7">
+      <c r="A59" t="s" s="5">
         <v>167</v>
       </c>
-      <c r="B59" t="s" s="8">
+      <c r="B59" t="s" s="6">
         <v>168</v>
       </c>
-      <c r="C59" t="s" s="29">
+      <c r="C59" t="s" s="23">
         <v>169</v>
       </c>
-      <c r="D59" s="10"/>
-      <c r="E59" s="11"/>
     </row>
     <row r="60" ht="31.5" customHeight="1">
-      <c r="A60" t="s" s="7">
+      <c r="A60" t="s" s="5">
         <v>170</v>
       </c>
-      <c r="B60" t="s" s="8">
+      <c r="B60" t="s" s="6">
         <v>171</v>
       </c>
-      <c r="C60" t="s" s="13">
+      <c r="C60" t="s" s="9">
         <v>172</v>
       </c>
-      <c r="D60" s="10"/>
-      <c r="E60" s="11"/>
     </row>
     <row r="61" ht="31.5" customHeight="1">
-      <c r="A61" t="s" s="7">
+      <c r="A61" t="s" s="5">
         <v>173</v>
       </c>
-      <c r="B61" t="s" s="8">
+      <c r="B61" t="s" s="6">
         <v>174</v>
       </c>
-      <c r="C61" t="s" s="13">
+      <c r="C61" t="s" s="9">
         <v>175</v>
       </c>
-      <c r="D61" s="10"/>
-      <c r="E61" s="11"/>
     </row>
     <row r="62" ht="54.75" customHeight="1">
-      <c r="A62" t="s" s="7">
+      <c r="A62" t="s" s="5">
         <v>176</v>
       </c>
-      <c r="B62" t="s" s="8">
+      <c r="B62" t="s" s="6">
         <v>177</v>
       </c>
-      <c r="C62" t="s" s="15">
+      <c r="C62" t="s" s="11">
         <v>178</v>
       </c>
-      <c r="D62" s="10"/>
-      <c r="E62" s="11"/>
     </row>
     <row r="63" ht="69.5" customHeight="1">
-      <c r="A63" t="s" s="7">
+      <c r="A63" t="s" s="5">
         <v>179</v>
       </c>
-      <c r="B63" t="s" s="8">
+      <c r="B63" t="s" s="6">
         <v>180</v>
       </c>
-      <c r="C63" t="s" s="16">
+      <c r="C63" t="s" s="12">
         <v>181</v>
       </c>
-      <c r="D63" s="10"/>
-      <c r="E63" s="11"/>
     </row>
     <row r="64" ht="46.75" customHeight="1">
-      <c r="A64" t="s" s="7">
+      <c r="A64" t="s" s="5">
         <v>182</v>
       </c>
-      <c r="B64" t="s" s="8">
+      <c r="B64" t="s" s="6">
         <v>183</v>
       </c>
-      <c r="C64" t="s" s="17">
+      <c r="C64" t="s" s="13">
         <v>184</v>
       </c>
-      <c r="D64" s="18"/>
-      <c r="E64" s="11"/>
     </row>
     <row r="65" ht="69.5" customHeight="1">
-      <c r="A65" t="s" s="7">
+      <c r="A65" t="s" s="5">
         <v>185</v>
       </c>
-      <c r="B65" t="s" s="8">
+      <c r="B65" t="s" s="6">
         <v>186</v>
       </c>
-      <c r="C65" t="s" s="13">
+      <c r="C65" t="s" s="9">
         <v>187</v>
       </c>
-      <c r="D65" s="10"/>
-      <c r="E65" s="11"/>
     </row>
     <row r="66" ht="106.5" customHeight="1">
-      <c r="A66" t="s" s="7">
+      <c r="A66" t="s" s="5">
         <v>188</v>
       </c>
-      <c r="B66" t="s" s="8">
+      <c r="B66" t="s" s="6">
         <v>189</v>
       </c>
-      <c r="C66" t="s" s="13">
+      <c r="C66" t="s" s="9">
         <v>190</v>
       </c>
-      <c r="D66" s="10"/>
-      <c r="E66" s="11"/>
     </row>
     <row r="67" ht="106.5" customHeight="1">
-      <c r="A67" t="s" s="7">
+      <c r="A67" t="s" s="5">
         <v>191</v>
       </c>
-      <c r="B67" t="s" s="8">
+      <c r="B67" t="s" s="6">
         <v>189</v>
       </c>
-      <c r="C67" t="s" s="13">
+      <c r="C67" t="s" s="9">
         <v>192</v>
       </c>
-      <c r="D67" s="10"/>
-      <c r="E67" s="11"/>
     </row>
     <row r="68" ht="31.5" customHeight="1">
-      <c r="A68" t="s" s="7">
+      <c r="A68" t="s" s="5">
         <v>193</v>
       </c>
-      <c r="B68" t="s" s="8">
+      <c r="B68" t="s" s="6">
         <v>186</v>
       </c>
-      <c r="C68" t="s" s="13">
+      <c r="C68" t="s" s="9">
         <v>194</v>
       </c>
-      <c r="D68" s="10"/>
-      <c r="E68" s="11"/>
     </row>
     <row r="69" ht="31.5" customHeight="1">
-      <c r="A69" t="s" s="7">
+      <c r="A69" t="s" s="5">
         <v>195</v>
       </c>
-      <c r="B69" t="s" s="8">
+      <c r="B69" t="s" s="6">
         <v>196</v>
       </c>
-      <c r="C69" t="s" s="13">
+      <c r="C69" t="s" s="9">
         <v>197</v>
       </c>
-      <c r="D69" s="10"/>
-      <c r="E69" s="11"/>
     </row>
     <row r="70" ht="69.75" customHeight="1">
-      <c r="A70" t="s" s="7">
+      <c r="A70" t="s" s="5">
         <v>198</v>
       </c>
-      <c r="B70" t="s" s="8">
+      <c r="B70" t="s" s="6">
         <v>199</v>
       </c>
-      <c r="C70" t="s" s="30">
+      <c r="C70" t="s" s="24">
         <v>200</v>
       </c>
-      <c r="D70" s="18"/>
-      <c r="E70" s="11"/>
     </row>
     <row r="71" ht="46.5" customHeight="1">
-      <c r="A71" t="s" s="7">
+      <c r="A71" t="s" s="5">
         <v>201</v>
       </c>
-      <c r="B71" t="s" s="8">
+      <c r="B71" t="s" s="6">
         <v>119</v>
       </c>
-      <c r="C71" t="s" s="31">
+      <c r="C71" t="s" s="25">
         <v>202</v>
       </c>
-      <c r="D71" s="18"/>
-      <c r="E71" s="11"/>
     </row>
     <row r="72" ht="54.75" customHeight="1">
-      <c r="A72" t="s" s="7">
+      <c r="A72" t="s" s="5">
         <v>203</v>
       </c>
-      <c r="B72" t="s" s="26">
+      <c r="B72" t="s" s="21">
         <v>204</v>
       </c>
-      <c r="C72" t="s" s="27">
+      <c r="C72" t="s" s="22">
         <v>205</v>
       </c>
-      <c r="D72" s="28"/>
-      <c r="E72" s="11"/>
     </row>
     <row r="73" ht="164.75" customHeight="1">
-      <c r="A73" t="s" s="7">
+      <c r="A73" t="s" s="5">
         <v>206</v>
       </c>
-      <c r="B73" t="s" s="8">
+      <c r="B73" t="s" s="6">
         <v>207</v>
       </c>
-      <c r="C73" t="s" s="32">
+      <c r="C73" t="s" s="26">
         <v>208</v>
       </c>
-      <c r="D73" s="10"/>
-      <c r="E73" s="11"/>
     </row>
     <row r="74" ht="77.75" customHeight="1">
-      <c r="A74" t="s" s="7">
+      <c r="A74" t="s" s="5">
         <v>209</v>
       </c>
-      <c r="B74" t="s" s="8">
+      <c r="B74" t="s" s="6">
         <v>210</v>
       </c>
-      <c r="C74" t="s" s="16">
+      <c r="C74" t="s" s="12">
         <v>211</v>
       </c>
-      <c r="D74" s="10"/>
-      <c r="E74" s="11"/>
     </row>
     <row r="75" ht="164.75" customHeight="1">
-      <c r="A75" t="s" s="7">
+      <c r="A75" t="s" s="5">
         <v>212</v>
       </c>
-      <c r="B75" t="s" s="8">
+      <c r="B75" t="s" s="6">
         <v>213</v>
       </c>
-      <c r="C75" t="s" s="16">
+      <c r="C75" t="s" s="12">
         <v>208</v>
       </c>
-      <c r="D75" s="10"/>
-      <c r="E75" s="11"/>
     </row>
     <row r="76" ht="164.75" customHeight="1">
-      <c r="A76" t="s" s="7">
+      <c r="A76" t="s" s="5">
         <v>214</v>
       </c>
-      <c r="B76" t="s" s="8">
+      <c r="B76" t="s" s="6">
         <v>215</v>
       </c>
-      <c r="C76" t="s" s="9">
+      <c r="C76" t="s" s="7">
         <v>216</v>
       </c>
-      <c r="D76" s="10"/>
-      <c r="E76" s="11"/>
     </row>
     <row r="77" ht="69.75" customHeight="1">
-      <c r="A77" t="s" s="7">
+      <c r="A77" t="s" s="5">
         <v>217</v>
       </c>
-      <c r="B77" t="s" s="8">
+      <c r="B77" t="s" s="6">
         <v>59</v>
       </c>
-      <c r="C77" t="s" s="17">
+      <c r="C77" t="s" s="13">
         <v>218</v>
       </c>
-      <c r="D77" s="18"/>
-      <c r="E77" s="11"/>
     </row>
     <row r="78" ht="77.75" customHeight="1">
-      <c r="A78" t="s" s="7">
+      <c r="A78" t="s" s="5">
         <v>219</v>
       </c>
-      <c r="B78" t="s" s="8">
+      <c r="B78" t="s" s="6">
         <v>220</v>
       </c>
-      <c r="C78" t="s" s="16">
+      <c r="C78" t="s" s="12">
         <v>221</v>
       </c>
-      <c r="D78" s="10"/>
-      <c r="E78" s="11"/>
     </row>
     <row r="79" ht="54.75" customHeight="1">
-      <c r="A79" t="s" s="7">
+      <c r="A79" t="s" s="5">
         <v>222</v>
       </c>
-      <c r="B79" t="s" s="8">
+      <c r="B79" t="s" s="6">
         <v>223</v>
       </c>
-      <c r="C79" t="s" s="16">
+      <c r="C79" t="s" s="12">
         <v>224</v>
       </c>
-      <c r="D79" s="10"/>
-      <c r="E79" s="11"/>
     </row>
     <row r="80" ht="46.5" customHeight="1">
-      <c r="A80" t="s" s="7">
+      <c r="A80" t="s" s="5">
         <v>225</v>
       </c>
-      <c r="B80" t="s" s="8">
+      <c r="B80" t="s" s="6">
         <v>226</v>
       </c>
-      <c r="C80" t="s" s="16">
+      <c r="C80" t="s" s="12">
         <v>227</v>
       </c>
-      <c r="D80" s="10"/>
-      <c r="E80" s="11"/>
     </row>
     <row r="81" ht="31.5" customHeight="1">
-      <c r="A81" t="s" s="7">
+      <c r="A81" t="s" s="5">
         <v>228</v>
       </c>
-      <c r="B81" t="s" s="8">
+      <c r="B81" t="s" s="6">
         <v>229</v>
       </c>
-      <c r="C81" t="s" s="33">
+      <c r="C81" t="s" s="27">
         <v>230</v>
       </c>
-      <c r="D81" s="18"/>
-      <c r="E81" s="11"/>
     </row>
     <row r="82" ht="77.75" customHeight="1">
-      <c r="A82" t="s" s="7">
+      <c r="A82" t="s" s="5">
         <v>231</v>
       </c>
-      <c r="B82" t="s" s="8">
+      <c r="B82" t="s" s="6">
         <v>232</v>
       </c>
-      <c r="C82" t="s" s="24">
+      <c r="C82" t="s" s="19">
         <v>43</v>
       </c>
-      <c r="D82" s="18"/>
-      <c r="E82" s="11"/>
     </row>
     <row r="83" ht="31.5" customHeight="1">
-      <c r="A83" t="s" s="7">
+      <c r="A83" t="s" s="5">
         <v>233</v>
       </c>
-      <c r="B83" t="s" s="8">
+      <c r="B83" t="s" s="6">
         <v>234</v>
       </c>
-      <c r="C83" t="s" s="15">
+      <c r="C83" t="s" s="11">
         <v>235</v>
       </c>
-      <c r="D83" s="10"/>
-      <c r="E83" s="11"/>
     </row>
     <row r="84" ht="31.5" customHeight="1">
-      <c r="A84" t="s" s="7">
+      <c r="A84" t="s" s="5">
         <v>236</v>
       </c>
-      <c r="B84" t="s" s="8">
+      <c r="B84" t="s" s="6">
         <v>237</v>
       </c>
-      <c r="C84" t="s" s="16">
+      <c r="C84" t="s" s="12">
         <v>238</v>
       </c>
-      <c r="D84" s="10"/>
-      <c r="E84" s="11"/>
     </row>
     <row r="85" ht="54.5" customHeight="1">
-      <c r="A85" t="s" s="7">
+      <c r="A85" t="s" s="5">
         <v>239</v>
       </c>
-      <c r="B85" t="s" s="8">
+      <c r="B85" t="s" s="6">
         <v>240</v>
       </c>
-      <c r="C85" t="s" s="9">
+      <c r="C85" t="s" s="7">
         <v>241</v>
       </c>
-      <c r="D85" s="10"/>
-      <c r="E85" s="11"/>
     </row>
     <row r="86" ht="409.5" customHeight="1">
-      <c r="A86" t="s" s="7">
+      <c r="A86" t="s" s="5">
         <v>242</v>
       </c>
-      <c r="B86" t="s" s="8">
+      <c r="B86" t="s" s="6">
         <v>243</v>
       </c>
-      <c r="C86" t="s" s="16">
+      <c r="C86" t="s" s="12">
         <v>244</v>
       </c>
-      <c r="D86" s="10"/>
-      <c r="E86" s="11"/>
     </row>
     <row r="87" ht="54.75" customHeight="1">
-      <c r="A87" t="s" s="7">
+      <c r="A87" t="s" s="5">
         <v>245</v>
       </c>
-      <c r="B87" t="s" s="8">
+      <c r="B87" t="s" s="6">
         <v>246</v>
       </c>
-      <c r="C87" t="s" s="22">
+      <c r="C87" t="s" s="17">
         <v>43</v>
       </c>
-      <c r="D87" s="18"/>
-      <c r="E87" s="11"/>
     </row>
     <row r="88" ht="46.75" customHeight="1">
-      <c r="A88" t="s" s="7">
+      <c r="A88" t="s" s="5">
         <v>247</v>
       </c>
-      <c r="B88" t="s" s="8">
+      <c r="B88" t="s" s="6">
         <v>248</v>
       </c>
-      <c r="C88" t="s" s="24">
+      <c r="C88" t="s" s="19">
         <v>249</v>
       </c>
-      <c r="D88" s="18"/>
-      <c r="E88" s="11"/>
     </row>
     <row r="89" ht="54.75" customHeight="1">
-      <c r="A89" t="s" s="7">
+      <c r="A89" t="s" s="5">
         <v>250</v>
       </c>
-      <c r="B89" t="s" s="8">
+      <c r="B89" t="s" s="6">
         <v>251</v>
       </c>
-      <c r="C89" t="s" s="15">
+      <c r="C89" t="s" s="11">
         <v>252</v>
       </c>
-      <c r="D89" s="10"/>
-      <c r="E89" s="11"/>
     </row>
     <row r="90" ht="54.5" customHeight="1">
-      <c r="A90" t="s" s="7">
+      <c r="A90" t="s" s="5">
         <v>253</v>
       </c>
-      <c r="B90" t="s" s="8">
+      <c r="B90" t="s" s="6">
         <v>254</v>
       </c>
-      <c r="C90" t="s" s="9">
+      <c r="C90" t="s" s="7">
         <v>255</v>
       </c>
-      <c r="D90" s="10"/>
-      <c r="E90" s="11"/>
     </row>
     <row r="91" ht="31.5" customHeight="1">
-      <c r="A91" t="s" s="7">
+      <c r="A91" t="s" s="5">
         <v>256</v>
       </c>
-      <c r="B91" t="s" s="8">
+      <c r="B91" t="s" s="6">
         <v>257</v>
       </c>
-      <c r="C91" t="s" s="8">
+      <c r="C91" t="s" s="6">
         <v>258</v>
       </c>
-      <c r="D91" s="10"/>
-      <c r="E91" s="11"/>
     </row>
     <row r="92" ht="46.75" customHeight="1">
-      <c r="A92" t="s" s="7">
+      <c r="A92" t="s" s="5">
         <v>259</v>
       </c>
-      <c r="B92" t="s" s="8">
+      <c r="B92" t="s" s="6">
         <v>260</v>
       </c>
-      <c r="C92" t="s" s="13">
+      <c r="C92" t="s" s="9">
         <v>261</v>
       </c>
-      <c r="D92" s="10"/>
-      <c r="E92" s="11"/>
     </row>
     <row r="93" ht="46.75" customHeight="1">
-      <c r="A93" t="s" s="7">
+      <c r="A93" t="s" s="5">
         <v>262</v>
       </c>
-      <c r="B93" t="s" s="8">
+      <c r="B93" t="s" s="6">
         <v>263</v>
       </c>
-      <c r="C93" t="s" s="16">
+      <c r="C93" t="s" s="12">
         <v>264</v>
       </c>
-      <c r="D93" s="10"/>
-      <c r="E93" s="11"/>
     </row>
     <row r="94" ht="46.75" customHeight="1">
-      <c r="A94" t="s" s="7">
+      <c r="A94" t="s" s="5">
         <v>265</v>
       </c>
-      <c r="B94" t="s" s="8">
+      <c r="B94" t="s" s="6">
         <v>266</v>
       </c>
-      <c r="C94" t="s" s="15">
+      <c r="C94" t="s" s="11">
         <v>267</v>
       </c>
-      <c r="D94" s="10"/>
-      <c r="E94" s="11"/>
     </row>
     <row r="95" ht="46.75" customHeight="1">
-      <c r="A95" t="s" s="7">
+      <c r="A95" t="s" s="5">
         <v>268</v>
       </c>
-      <c r="B95" t="s" s="8">
+      <c r="B95" t="s" s="6">
         <v>269</v>
       </c>
-      <c r="C95" t="s" s="15">
+      <c r="C95" t="s" s="11">
         <v>270</v>
       </c>
-      <c r="D95" s="10"/>
-      <c r="E95" s="11"/>
     </row>
     <row r="96" ht="46.5" customHeight="1">
-      <c r="A96" t="s" s="7">
+      <c r="A96" t="s" s="5">
         <v>271</v>
       </c>
-      <c r="B96" t="s" s="8">
+      <c r="B96" t="s" s="6">
         <v>272</v>
       </c>
-      <c r="C96" t="s" s="16">
+      <c r="C96" t="s" s="12">
         <v>273</v>
       </c>
-      <c r="D96" s="10"/>
-      <c r="E96" s="11"/>
     </row>
     <row r="97" ht="46.5" customHeight="1">
-      <c r="A97" t="s" s="7">
+      <c r="A97" t="s" s="5">
         <v>274</v>
       </c>
-      <c r="B97" t="s" s="8">
+      <c r="B97" t="s" s="6">
         <v>183</v>
       </c>
-      <c r="C97" t="s" s="17">
+      <c r="C97" t="s" s="13">
         <v>43</v>
       </c>
-      <c r="D97" s="18"/>
-      <c r="E97" s="11"/>
     </row>
     <row r="98" ht="46.5" customHeight="1">
-      <c r="A98" t="s" s="7">
+      <c r="A98" t="s" s="5">
         <v>275</v>
       </c>
-      <c r="B98" t="s" s="8">
+      <c r="B98" t="s" s="6">
         <v>276</v>
       </c>
-      <c r="C98" t="s" s="16">
+      <c r="C98" t="s" s="12">
         <v>277</v>
       </c>
-      <c r="D98" s="10"/>
-      <c r="E98" s="11"/>
     </row>
     <row r="99" ht="46.75" customHeight="1">
-      <c r="A99" t="s" s="7">
+      <c r="A99" t="s" s="5">
         <v>278</v>
       </c>
-      <c r="B99" t="s" s="8">
+      <c r="B99" t="s" s="6">
         <v>279</v>
       </c>
-      <c r="C99" t="s" s="15">
+      <c r="C99" t="s" s="11">
         <v>280</v>
       </c>
-      <c r="D99" s="10"/>
-      <c r="E99" s="11"/>
     </row>
     <row r="100" ht="15" customHeight="1">
-      <c r="A100" t="s" s="34">
+      <c r="A100" t="s" s="28">
         <v>281</v>
       </c>
-      <c r="B100" t="s" s="35">
+      <c r="B100" t="s" s="29">
         <v>282</v>
       </c>
-      <c r="C100" t="s" s="36">
+      <c r="C100" t="s" s="30">
         <v>283</v>
       </c>
-      <c r="D100" s="37"/>
-      <c r="E100" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>